<commit_message>
Update Ofertas de Disciplinas - UFMG PPGCC.xlsx
</commit_message>
<xml_diff>
--- a/Files/Disciplinas/Ofertas de Disciplinas - UFMG PPGCC.xlsx
+++ b/Files/Disciplinas/Ofertas de Disciplinas - UFMG PPGCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\UFMG\MiscDocs_PPGCC\Files\Disciplinas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D861CA6-50DD-45B8-AF76-545D9038A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7DB5CE-AE02-494D-9592-A37EFFECDD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="980" firstSheet="2" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9082" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9083" uniqueCount="1075">
   <si>
     <t>Nome da Atividade</t>
   </si>
@@ -3233,22 +3233,6 @@
   </si>
   <si>
     <t>cancelada</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TECC: Bancos de Dados Geográficos
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Godovesi Davái</t>
-    </r>
   </si>
   <si>
     <r>
@@ -3264,22 +3248,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Flávio</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TECC: Métodos Formais
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Hamiel</t>
     </r>
   </si>
   <si>
@@ -3702,12 +3670,44 @@
       <t>Ítalo</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TECC: Métodos Formais
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Haniel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TECC: Bancos de Dados Geográficos
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clodoveu Davis</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3849,6 +3849,13 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -4564,7 +4571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5071,7 +5078,12 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -5250,7 +5262,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -11550,7 +11562,7 @@
     <tableColumn id="6" xr3:uid="{810BEAB3-711C-4133-9BA3-3A7D37EFC94C}" name="QUI" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{68739D62-0C71-48FE-88CA-95B7A45FA9D7}" name="SEX" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -50558,7 +50570,7 @@
     <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="220.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="210" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="155" t="s">
         <v>783</v>
       </c>
@@ -52126,14 +52138,14 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" customWidth="1"/>
@@ -52155,22 +52167,22 @@
     </row>
     <row r="2" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="190" t="s">
         <v>1001</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="191" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="191" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="191" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="191" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="191" t="s">
         <v>102</v>
       </c>
       <c r="H2" s="1"/>
@@ -52182,11 +52194,11 @@
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="38" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="38" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="G3" s="180"/>
       <c r="H3" s="1"/>
@@ -52198,11 +52210,11 @@
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="37" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="37" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="G4" s="181"/>
       <c r="H4" s="1"/>
@@ -52214,11 +52226,11 @@
       </c>
       <c r="C5" s="138"/>
       <c r="D5" s="138" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="E5" s="138"/>
       <c r="F5" s="138" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="G5" s="182"/>
       <c r="H5" s="1"/>
@@ -52229,19 +52241,19 @@
         <v>109</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>1046</v>
+        <v>1074</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>1046</v>
+        <v>1074</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="G6" s="183" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -52251,19 +52263,19 @@
         <v>109</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="G7" s="183" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -52273,16 +52285,16 @@
         <v>109</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>1048</v>
+        <v>1073</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>1048</v>
+        <v>1073</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="G8" s="183"/>
       <c r="H8" s="1"/>
@@ -52293,11 +52305,11 @@
         <v>109</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D9" s="41"/>
       <c r="E9" s="41" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="183"/>
@@ -52309,16 +52321,16 @@
         <v>110</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G10" s="184"/>
       <c r="H10" s="1"/>
@@ -52329,16 +52341,16 @@
         <v>110</v>
       </c>
       <c r="C11" s="43" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D11" s="43" t="s">
         <v>1056</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>1058</v>
-      </c>
       <c r="E11" s="43" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F11" s="43" t="s">
         <v>1056</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>1058</v>
       </c>
       <c r="G11" s="184"/>
       <c r="H11" s="1"/>
@@ -52352,7 +52364,7 @@
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
       <c r="F12" s="43" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="G12" s="184"/>
       <c r="H12" s="1"/>
@@ -52363,16 +52375,16 @@
         <v>111</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="F13" s="45" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="G13" s="185"/>
       <c r="H13" s="1"/>
@@ -52383,16 +52395,16 @@
         <v>111</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="F14" s="45" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="G14" s="185"/>
       <c r="H14" s="1"/>
@@ -52403,16 +52415,16 @@
         <v>111</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="F15" s="45" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="G15" s="185"/>
       <c r="H15" s="1"/>
@@ -52423,16 +52435,16 @@
         <v>111</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E16" s="45" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="F16" s="45" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="G16" s="185"/>
       <c r="H16" s="1"/>
@@ -52443,16 +52455,16 @@
         <v>111</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E17" s="45" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="F17" s="45" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="G17" s="185"/>
       <c r="H17" s="1"/>
@@ -52463,10 +52475,12 @@
         <v>112</v>
       </c>
       <c r="C18" s="187" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D18" s="188"/>
-      <c r="E18" s="188"/>
+      <c r="E18" s="187" t="s">
+        <v>1059</v>
+      </c>
       <c r="F18" s="188"/>
       <c r="G18" s="189"/>
       <c r="H18" s="1"/>
@@ -52499,9 +52513,9 @@
       <c r="A21" s="1"/>
       <c r="B21" s="126"/>
       <c r="C21" s="131" t="s">
-        <v>1073</v>
-      </c>
-      <c r="D21" s="190" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D21" s="179" t="s">
         <v>1009</v>
       </c>
       <c r="E21" s="126"/>

</xml_diff>